<commit_message>
add new code for reading excel file and fix issues about columns but need to handle missing columns in csv
</commit_message>
<xml_diff>
--- a/diabetes.xlsx
+++ b/diabetes.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eng\Desktop\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1CB12E3-9511-4D19-95B6-E00933E600B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C7E70BD4-C2D6-4A4D-968F-C353F90A08FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="diabetes" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -891,11 +891,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I769"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I4"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>